<commit_message>
updated image to render better
</commit_message>
<xml_diff>
--- a/o-23/data/Construction Spending - Data 2025 04 01.xlsx
+++ b/o-23/data/Construction Spending - Data 2025 04 01.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\C30\ProcessingNew\Final Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shaurya\lab\The-Silmaril\o-23\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC6B2CC-1C0B-4C86-A03A-4DB0E5F44D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15225" yWindow="-15495" windowWidth="21615" windowHeight="14775" xr2:uid="{E4F6DD96-F975-499A-AAF4-2188A7762B8C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="3744"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="4" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Table3!$A$1:$F$71</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="85">
   <si>
     <t>(Millions of dollars. Details may not add to totals due to rounding.)</t>
   </si>
@@ -368,10 +367,6 @@
   <si>
     <t xml:space="preserve">            Type of Construction
 </t>
-  </si>
-  <si>
-    <t>Jan
-2025</t>
   </si>
   <si>
     <t>Data are at an annual rate, adjusted for seasonality but not price changes. Source: U.S. Census Bureau, Construction Spending, April 1, 2025.</t>
@@ -613,13 +608,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,###"/>
     <numFmt numFmtId="165" formatCode="##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -871,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1014,6 +1009,18 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1348,24 +1355,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289F3768-76A2-4201-883B-F32239A4B2F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection sqref="A1:I79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="9.9" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="27" customWidth="1"/>
-    <col min="2" max="7" width="8.28515625" style="24" customWidth="1"/>
-    <col min="8" max="9" width="8.28515625" style="26" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="26.69921875" style="27" customWidth="1"/>
+    <col min="2" max="7" width="8.296875" style="24" customWidth="1"/>
+    <col min="8" max="9" width="8.296875" style="26" customWidth="1"/>
+    <col min="10" max="16384" width="9.09765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -1376,7 +1383,7 @@
       <c r="H1" s="46"/>
       <c r="I1" s="46"/>
     </row>
-    <row r="2" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="9.75" customHeight="1">
       <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1396,7 @@
       <c r="H2" s="47"/>
       <c r="I2" s="47"/>
     </row>
-    <row r="3" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="7.5" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1400,7 +1407,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="21.9" customHeight="1">
       <c r="A4" s="28"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -1411,38 +1418,38 @@
       <c r="H4" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="48"/>
-    </row>
-    <row r="5" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="55"/>
+    </row>
+    <row r="5" spans="1:9" ht="26.25" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="52">
+        <v>45689</v>
+      </c>
+      <c r="C5" s="52">
+        <v>45658</v>
+      </c>
+      <c r="D5" s="52">
+        <v>45627</v>
+      </c>
+      <c r="E5" s="52">
+        <v>45597</v>
+      </c>
+      <c r="F5" s="52">
+        <v>45566</v>
+      </c>
+      <c r="G5" s="53">
+        <v>45323</v>
+      </c>
+      <c r="H5" s="54">
+        <v>45658</v>
+      </c>
+      <c r="I5" s="54">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="7.5" customHeight="1">
       <c r="A6" s="32"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1453,7 +1460,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" s="17" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="17" customFormat="1" ht="9.9" customHeight="1">
       <c r="A7" s="33" t="s">
         <v>5</v>
       </c>
@@ -1482,7 +1489,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="4.5" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1493,7 +1500,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="9.9" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>6</v>
       </c>
@@ -1522,7 +1529,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="4.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -1533,7 +1540,7 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="9.9" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>7</v>
       </c>
@@ -1562,7 +1569,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="9.9" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>8</v>
       </c>
@@ -1591,7 +1598,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="9.9" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>9</v>
       </c>
@@ -1620,7 +1627,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="9.9" customHeight="1">
       <c r="A14" s="32" t="s">
         <v>10</v>
       </c>
@@ -1649,7 +1656,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="9.9" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>11</v>
       </c>
@@ -1678,7 +1685,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="9.9" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>12</v>
       </c>
@@ -1707,7 +1714,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="9.9" customHeight="1">
       <c r="A17" s="32" t="s">
         <v>13</v>
       </c>
@@ -1736,7 +1743,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="9.9" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>14</v>
       </c>
@@ -1765,7 +1772,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="9.9" customHeight="1">
       <c r="A19" s="32" t="s">
         <v>15</v>
       </c>
@@ -1794,7 +1801,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="9.9" customHeight="1">
       <c r="A20" s="32" t="s">
         <v>16</v>
       </c>
@@ -1823,7 +1830,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="9.9" customHeight="1">
       <c r="A21" s="32" t="s">
         <v>17</v>
       </c>
@@ -1852,7 +1859,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="9.9" customHeight="1">
       <c r="A22" s="32" t="s">
         <v>18</v>
       </c>
@@ -1881,7 +1888,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="9.9" customHeight="1">
       <c r="A23" s="32" t="s">
         <v>19</v>
       </c>
@@ -1910,7 +1917,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="9.9" customHeight="1">
       <c r="A24" s="32" t="s">
         <v>20</v>
       </c>
@@ -1939,7 +1946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="9.9" customHeight="1">
       <c r="A25" s="32" t="s">
         <v>21</v>
       </c>
@@ -1968,7 +1975,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="9.9" customHeight="1">
       <c r="A26" s="32" t="s">
         <v>22</v>
       </c>
@@ -1997,7 +2004,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="9.9" customHeight="1">
       <c r="A27" s="32" t="s">
         <v>23</v>
       </c>
@@ -2026,7 +2033,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="4.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -2037,9 +2044,9 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" s="17" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" s="17" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="15">
         <v>1686409</v>
@@ -2066,7 +2073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="4.5" customHeight="1">
       <c r="A30" s="32"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -2077,9 +2084,9 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12" customHeight="1">
       <c r="A31" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="11">
         <v>928893</v>
@@ -2106,7 +2113,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="9.9" customHeight="1">
       <c r="A32" s="32" t="s">
         <v>27</v>
       </c>
@@ -2135,7 +2142,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="9.9" customHeight="1">
       <c r="A33" s="32" t="s">
         <v>28</v>
       </c>
@@ -2164,7 +2171,7 @@
         <v>-11.6</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="4.5" customHeight="1">
       <c r="A34" s="32"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -2175,7 +2182,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="9.9" customHeight="1">
       <c r="A35" s="32" t="s">
         <v>7</v>
       </c>
@@ -2204,7 +2211,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="9.9" customHeight="1">
       <c r="A36" s="32" t="s">
         <v>8</v>
       </c>
@@ -2233,7 +2240,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="9.9" customHeight="1">
       <c r="A37" s="32" t="s">
         <v>9</v>
       </c>
@@ -2262,7 +2269,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="9.9" customHeight="1">
       <c r="A38" s="32" t="s">
         <v>10</v>
       </c>
@@ -2291,7 +2298,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="9.9" customHeight="1">
       <c r="A39" s="32" t="s">
         <v>29</v>
       </c>
@@ -2320,7 +2327,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="9.9" customHeight="1">
       <c r="A40" s="32" t="s">
         <v>12</v>
       </c>
@@ -2349,7 +2356,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="9.9" customHeight="1">
       <c r="A41" s="32" t="s">
         <v>13</v>
       </c>
@@ -2378,7 +2385,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="9.9" customHeight="1">
       <c r="A42" s="32" t="s">
         <v>31</v>
       </c>
@@ -2407,7 +2414,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="9.9" customHeight="1">
       <c r="A43" s="32" t="s">
         <v>16</v>
       </c>
@@ -2436,7 +2443,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="9.9" customHeight="1">
       <c r="A44" s="32" t="s">
         <v>17</v>
       </c>
@@ -2465,7 +2472,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="9.9" customHeight="1">
       <c r="A45" s="32" t="s">
         <v>18</v>
       </c>
@@ -2494,7 +2501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="9.9" customHeight="1">
       <c r="A46" s="32" t="s">
         <v>55</v>
       </c>
@@ -2523,7 +2530,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="4.5" customHeight="1">
       <c r="A47" s="32"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -2534,9 +2541,9 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" s="17" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" s="17" customFormat="1" ht="12" customHeight="1">
       <c r="A48" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="15">
         <v>509346</v>
@@ -2563,7 +2570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="4.5" customHeight="1">
       <c r="A49" s="32"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -2574,7 +2581,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="9.9" customHeight="1">
       <c r="A50" s="32" t="s">
         <v>6</v>
       </c>
@@ -2603,7 +2610,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="4.5" customHeight="1">
       <c r="A51" s="32"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -2614,7 +2621,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="9.9" customHeight="1">
       <c r="A52" s="32" t="s">
         <v>7</v>
       </c>
@@ -2643,7 +2650,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="9.9" customHeight="1">
       <c r="A53" s="32" t="s">
         <v>9</v>
       </c>
@@ -2672,7 +2679,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="9.9" customHeight="1">
       <c r="A54" s="32" t="s">
         <v>10</v>
       </c>
@@ -2701,7 +2708,7 @@
         <v>53.1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="9.9" customHeight="1">
       <c r="A55" s="32" t="s">
         <v>29</v>
       </c>
@@ -2730,7 +2737,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="9.9" customHeight="1">
       <c r="A56" s="32" t="s">
         <v>12</v>
       </c>
@@ -2759,7 +2766,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="9.9" customHeight="1">
       <c r="A57" s="32" t="s">
         <v>14</v>
       </c>
@@ -2788,7 +2795,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="9.9" customHeight="1">
       <c r="A58" s="32" t="s">
         <v>15</v>
       </c>
@@ -2817,7 +2824,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="9.9" customHeight="1">
       <c r="A59" s="32" t="s">
         <v>16</v>
       </c>
@@ -2846,7 +2853,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="9.9" customHeight="1">
       <c r="A60" s="32" t="s">
         <v>18</v>
       </c>
@@ -2875,7 +2882,7 @@
         <v>-7.1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="9.9" customHeight="1">
       <c r="A61" s="32" t="s">
         <v>36</v>
       </c>
@@ -2904,7 +2911,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="9.9" customHeight="1">
       <c r="A62" s="32" t="s">
         <v>20</v>
       </c>
@@ -2933,7 +2940,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="9.9" customHeight="1">
       <c r="A63" s="32" t="s">
         <v>33</v>
       </c>
@@ -2962,7 +2969,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="9.9" customHeight="1">
       <c r="A64" s="19" t="s">
         <v>37</v>
       </c>
@@ -2991,10 +2998,10 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="4.5" customHeight="1"/>
+    <row r="66" spans="1:9" ht="10.5" customHeight="1">
       <c r="A66" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="23"/>
       <c r="C66" s="23"/>
@@ -3005,7 +3012,7 @@
       <c r="H66" s="23"/>
       <c r="I66" s="23"/>
     </row>
-    <row r="67" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="4.5" customHeight="1">
       <c r="A67" s="22"/>
       <c r="B67" s="22"/>
       <c r="C67" s="22"/>
@@ -3016,9 +3023,9 @@
       <c r="H67" s="22"/>
       <c r="I67" s="22"/>
     </row>
-    <row r="68" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="10.5" customHeight="1">
       <c r="A68" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
@@ -3029,7 +3036,7 @@
       <c r="H68" s="23"/>
       <c r="I68" s="23"/>
     </row>
-    <row r="69" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="10.5" customHeight="1">
       <c r="A69" s="22" t="s">
         <v>64</v>
       </c>
@@ -3042,7 +3049,7 @@
       <c r="H69" s="22"/>
       <c r="I69" s="22"/>
     </row>
-    <row r="70" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="4.5" customHeight="1">
       <c r="A70" s="22"/>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
@@ -3053,9 +3060,9 @@
       <c r="H70" s="22"/>
       <c r="I70" s="22"/>
     </row>
-    <row r="71" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="10.5" customHeight="1">
       <c r="A71" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" s="23"/>
       <c r="C71" s="23"/>
@@ -3066,7 +3073,7 @@
       <c r="H71" s="23"/>
       <c r="I71" s="23"/>
     </row>
-    <row r="72" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="4.5" customHeight="1">
       <c r="A72" s="22"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
@@ -3077,9 +3084,9 @@
       <c r="H72" s="22"/>
       <c r="I72" s="22"/>
     </row>
-    <row r="73" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="10.5" customHeight="1">
       <c r="A73" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B73" s="23"/>
       <c r="C73" s="23"/>
@@ -3090,7 +3097,7 @@
       <c r="H73" s="23"/>
       <c r="I73" s="23"/>
     </row>
-    <row r="74" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="9" customHeight="1">
       <c r="A74" s="22" t="s">
         <v>43</v>
       </c>
@@ -3103,7 +3110,7 @@
       <c r="H74" s="22"/>
       <c r="I74" s="22"/>
     </row>
-    <row r="75" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="4.5" customHeight="1">
       <c r="A75" s="22"/>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
@@ -3114,9 +3121,9 @@
       <c r="H75" s="22"/>
       <c r="I75" s="22"/>
     </row>
-    <row r="76" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="9.9" customHeight="1">
       <c r="A76" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
@@ -3127,7 +3134,7 @@
       <c r="H76" s="22"/>
       <c r="I76" s="22"/>
     </row>
-    <row r="77" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="9.9" customHeight="1">
       <c r="A77" s="22" t="s">
         <v>66</v>
       </c>
@@ -3140,7 +3147,7 @@
       <c r="H77" s="22"/>
       <c r="I77" s="22"/>
     </row>
-    <row r="78" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="9.9" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>45</v>
       </c>
@@ -3160,7 +3167,7 @@
     <mergeCell ref="H4:I4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A78" r:id="rId1" tooltip="&lt;www.census.gov/construction/c30/meth.html&gt;" xr:uid="{1C68931A-7FF3-4AA1-B874-5A0E9812F0FD}"/>
+    <hyperlink ref="A78" r:id="rId1" tooltip="&lt;www.census.gov/construction/c30/meth.html&gt;"/>
   </hyperlinks>
   <pageMargins left="0.55555555555555558" right="0.55555555555555558" top="0.41666666666666669" bottom="0.1388888888888889" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3168,24 +3175,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD9B29A-3DAB-4C00-9643-E2B4FF100A4C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="9.9" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="27" customWidth="1"/>
-    <col min="2" max="9" width="7.7109375" style="24" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="26" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="26.69921875" style="27" customWidth="1"/>
+    <col min="2" max="9" width="7.69921875" style="24" customWidth="1"/>
+    <col min="10" max="10" width="7.69921875" style="26" customWidth="1"/>
+    <col min="11" max="16384" width="9.09765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="12.75" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -3197,7 +3204,7 @@
       <c r="I1" s="46"/>
       <c r="J1" s="46"/>
     </row>
-    <row r="2" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="9.75" customHeight="1">
       <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
@@ -3211,7 +3218,7 @@
       <c r="I2" s="47"/>
       <c r="J2" s="47"/>
     </row>
-    <row r="3" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="7.5" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3223,7 +3230,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="9.9" customHeight="1">
       <c r="A4" s="28"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -3237,18 +3244,18 @@
       <c r="I4" s="49"/>
       <c r="J4" s="49"/>
     </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="33" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="D5" s="20" t="s">
         <v>75</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>76</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>60</v>
@@ -3269,7 +3276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="7.5" customHeight="1">
       <c r="A6" s="32"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -3281,7 +3288,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" s="17" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="17" customFormat="1" ht="9.9" customHeight="1">
       <c r="A7" s="33" t="s">
         <v>5</v>
       </c>
@@ -3313,7 +3320,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="4.5" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -3325,7 +3332,7 @@
       <c r="I8" s="11"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="9.9" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>6</v>
       </c>
@@ -3357,7 +3364,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="4.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3369,7 +3376,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="9.9" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>7</v>
       </c>
@@ -3401,7 +3408,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="9.9" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>8</v>
       </c>
@@ -3433,7 +3440,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="9.9" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>9</v>
       </c>
@@ -3465,7 +3472,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="9.9" customHeight="1">
       <c r="A14" s="32" t="s">
         <v>10</v>
       </c>
@@ -3497,7 +3504,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="9.9" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>11</v>
       </c>
@@ -3529,7 +3536,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="9.9" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>12</v>
       </c>
@@ -3561,7 +3568,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="9.9" customHeight="1">
       <c r="A17" s="32" t="s">
         <v>13</v>
       </c>
@@ -3593,7 +3600,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="9.9" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>14</v>
       </c>
@@ -3625,7 +3632,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="9.9" customHeight="1">
       <c r="A19" s="32" t="s">
         <v>15</v>
       </c>
@@ -3657,7 +3664,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="9.9" customHeight="1">
       <c r="A20" s="32" t="s">
         <v>16</v>
       </c>
@@ -3689,7 +3696,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="9.9" customHeight="1">
       <c r="A21" s="32" t="s">
         <v>17</v>
       </c>
@@ -3721,7 +3728,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="9.9" customHeight="1">
       <c r="A22" s="32" t="s">
         <v>18</v>
       </c>
@@ -3753,7 +3760,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="9.9" customHeight="1">
       <c r="A23" s="32" t="s">
         <v>19</v>
       </c>
@@ -3785,7 +3792,7 @@
         <v>-1.9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="9.9" customHeight="1">
       <c r="A24" s="32" t="s">
         <v>20</v>
       </c>
@@ -3817,7 +3824,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="9.9" customHeight="1">
       <c r="A25" s="32" t="s">
         <v>21</v>
       </c>
@@ -3849,7 +3856,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="9.9" customHeight="1">
       <c r="A26" s="32" t="s">
         <v>22</v>
       </c>
@@ -3881,7 +3888,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="9.9" customHeight="1">
       <c r="A27" s="32" t="s">
         <v>23</v>
       </c>
@@ -3913,7 +3920,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="4.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -3925,9 +3932,9 @@
       <c r="I28" s="11"/>
       <c r="J28" s="13"/>
     </row>
-    <row r="29" spans="1:10" s="17" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="17" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="15">
         <v>122824</v>
@@ -3957,7 +3964,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="4.5" customHeight="1">
       <c r="A30" s="32"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -3969,9 +3976,9 @@
       <c r="I30" s="11"/>
       <c r="J30" s="13"/>
     </row>
-    <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="11">
         <v>64076</v>
@@ -4001,7 +4008,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="9.9" customHeight="1">
       <c r="A32" s="32" t="s">
         <v>27</v>
       </c>
@@ -4033,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="9.9" customHeight="1">
       <c r="A33" s="32" t="s">
         <v>28</v>
       </c>
@@ -4065,7 +4072,7 @@
         <v>-14.4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="4.5" customHeight="1">
       <c r="A34" s="32"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -4077,7 +4084,7 @@
       <c r="I34" s="11"/>
       <c r="J34" s="13"/>
     </row>
-    <row r="35" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="9.9" customHeight="1">
       <c r="A35" s="32" t="s">
         <v>7</v>
       </c>
@@ -4109,7 +4116,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="9.9" customHeight="1">
       <c r="A36" s="32" t="s">
         <v>8</v>
       </c>
@@ -4141,7 +4148,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="9.9" customHeight="1">
       <c r="A37" s="32" t="s">
         <v>9</v>
       </c>
@@ -4173,7 +4180,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="9.9" customHeight="1">
       <c r="A38" s="32" t="s">
         <v>10</v>
       </c>
@@ -4205,7 +4212,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="9.9" customHeight="1">
       <c r="A39" s="32" t="s">
         <v>29</v>
       </c>
@@ -4237,7 +4244,7 @@
         <v>-3.7</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="9.9" customHeight="1">
       <c r="A40" s="32" t="s">
         <v>12</v>
       </c>
@@ -4269,7 +4276,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="9.9" customHeight="1">
       <c r="A41" s="32" t="s">
         <v>13</v>
       </c>
@@ -4301,7 +4308,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="9.9" customHeight="1">
       <c r="A42" s="32" t="s">
         <v>31</v>
       </c>
@@ -4333,7 +4340,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="9.9" customHeight="1">
       <c r="A43" s="32" t="s">
         <v>16</v>
       </c>
@@ -4365,7 +4372,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="9.9" customHeight="1">
       <c r="A44" s="32" t="s">
         <v>17</v>
       </c>
@@ -4397,7 +4404,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="9.9" customHeight="1">
       <c r="A45" s="32" t="s">
         <v>18</v>
       </c>
@@ -4429,7 +4436,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="9.9" customHeight="1">
       <c r="A46" s="32" t="s">
         <v>55</v>
       </c>
@@ -4461,7 +4468,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="4.5" customHeight="1">
       <c r="A47" s="32"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -4473,9 +4480,9 @@
       <c r="I47" s="11"/>
       <c r="J47" s="13"/>
     </row>
-    <row r="48" spans="1:10" s="17" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" s="17" customFormat="1" ht="12" customHeight="1">
       <c r="A48" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="15">
         <v>33112</v>
@@ -4505,7 +4512,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="4.5" customHeight="1">
       <c r="A49" s="32"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -4517,7 +4524,7 @@
       <c r="I49" s="11"/>
       <c r="J49" s="13"/>
     </row>
-    <row r="50" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="9.9" customHeight="1">
       <c r="A50" s="32" t="s">
         <v>6</v>
       </c>
@@ -4549,7 +4556,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="4.5" customHeight="1">
       <c r="A51" s="32"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -4561,7 +4568,7 @@
       <c r="I51" s="11"/>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="9.9" customHeight="1">
       <c r="A52" s="32" t="s">
         <v>7</v>
       </c>
@@ -4593,7 +4600,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="9.9" customHeight="1">
       <c r="A53" s="32" t="s">
         <v>9</v>
       </c>
@@ -4625,7 +4632,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="9.9" customHeight="1">
       <c r="A54" s="32" t="s">
         <v>10</v>
       </c>
@@ -4657,7 +4664,7 @@
         <v>50.5</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="9.9" customHeight="1">
       <c r="A55" s="32" t="s">
         <v>29</v>
       </c>
@@ -4689,7 +4696,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="9.9" customHeight="1">
       <c r="A56" s="32" t="s">
         <v>12</v>
       </c>
@@ -4721,7 +4728,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="9.9" customHeight="1">
       <c r="A57" s="32" t="s">
         <v>14</v>
       </c>
@@ -4753,7 +4760,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="9.9" customHeight="1">
       <c r="A58" s="32" t="s">
         <v>15</v>
       </c>
@@ -4785,7 +4792,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="9.9" customHeight="1">
       <c r="A59" s="32" t="s">
         <v>16</v>
       </c>
@@ -4817,7 +4824,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="9.9" customHeight="1">
       <c r="A60" s="32" t="s">
         <v>18</v>
       </c>
@@ -4849,7 +4856,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="9.9" customHeight="1">
       <c r="A61" s="32" t="s">
         <v>36</v>
       </c>
@@ -4881,7 +4888,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" ht="9.9" customHeight="1">
       <c r="A62" s="32" t="s">
         <v>20</v>
       </c>
@@ -4913,7 +4920,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="9.9" customHeight="1">
       <c r="A63" s="32" t="s">
         <v>33</v>
       </c>
@@ -4945,7 +4952,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" ht="9.9" customHeight="1">
       <c r="A64" s="19" t="s">
         <v>37</v>
       </c>
@@ -4977,10 +4984,10 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="4.5" customHeight="1"/>
+    <row r="66" spans="1:10" ht="10.5" customHeight="1">
       <c r="A66" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="23"/>
       <c r="C66" s="23"/>
@@ -4992,7 +4999,7 @@
       <c r="I66" s="23"/>
       <c r="J66" s="23"/>
     </row>
-    <row r="67" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="4.5" customHeight="1">
       <c r="A67" s="22"/>
       <c r="B67" s="22"/>
       <c r="C67" s="22"/>
@@ -5004,9 +5011,9 @@
       <c r="I67" s="22"/>
       <c r="J67" s="34"/>
     </row>
-    <row r="68" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="10.5" customHeight="1">
       <c r="A68" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
@@ -5018,7 +5025,7 @@
       <c r="I68" s="23"/>
       <c r="J68" s="23"/>
     </row>
-    <row r="69" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="10.5" customHeight="1">
       <c r="A69" s="22" t="s">
         <v>64</v>
       </c>
@@ -5032,7 +5039,7 @@
       <c r="I69" s="22"/>
       <c r="J69" s="22"/>
     </row>
-    <row r="70" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="4.5" customHeight="1">
       <c r="A70" s="22"/>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
@@ -5044,9 +5051,9 @@
       <c r="I70" s="22"/>
       <c r="J70" s="34"/>
     </row>
-    <row r="71" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="10.5" customHeight="1">
       <c r="A71" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" s="23"/>
       <c r="C71" s="23"/>
@@ -5058,7 +5065,7 @@
       <c r="I71" s="23"/>
       <c r="J71" s="23"/>
     </row>
-    <row r="72" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="4.5" customHeight="1">
       <c r="A72" s="22"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
@@ -5070,9 +5077,9 @@
       <c r="I72" s="22"/>
       <c r="J72" s="34"/>
     </row>
-    <row r="73" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="10.5" customHeight="1">
       <c r="A73" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B73" s="23"/>
       <c r="C73" s="23"/>
@@ -5084,7 +5091,7 @@
       <c r="I73" s="23"/>
       <c r="J73" s="23"/>
     </row>
-    <row r="74" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="10.5" customHeight="1">
       <c r="A74" s="22" t="s">
         <v>43</v>
       </c>
@@ -5098,7 +5105,7 @@
       <c r="I74" s="22"/>
       <c r="J74" s="22"/>
     </row>
-    <row r="75" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="4.5" customHeight="1">
       <c r="A75" s="22"/>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
@@ -5110,7 +5117,7 @@
       <c r="I75" s="22"/>
       <c r="J75" s="34"/>
     </row>
-    <row r="76" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="10.5" customHeight="1">
       <c r="A76" s="22" t="s">
         <v>65</v>
       </c>
@@ -5124,7 +5131,7 @@
       <c r="I76" s="22"/>
       <c r="J76" s="22"/>
     </row>
-    <row r="77" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="10.5" customHeight="1">
       <c r="A77" s="22" t="s">
         <v>66</v>
       </c>
@@ -5138,7 +5145,7 @@
       <c r="I77" s="22"/>
       <c r="J77" s="22"/>
     </row>
-    <row r="78" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="10.5" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>45</v>
       </c>
@@ -5159,7 +5166,7 @@
     <mergeCell ref="H4:J4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A78" r:id="rId1" tooltip="&lt;www.census.gov/construction/c30/meth.html&gt;" xr:uid="{C7690EA6-78EA-4B7C-95F3-A9241B09ECAE}"/>
+    <hyperlink ref="A78" r:id="rId1" tooltip="&lt;www.census.gov/construction/c30/meth.html&gt;"/>
   </hyperlinks>
   <pageMargins left="0.55555555555555558" right="0.27777777777777779" top="0.41666666666666669" bottom="0.1388888888888889" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5167,23 +5174,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79C5B85-CB1B-4DC3-9162-BFC4B0273C2B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="9.9" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="27" customWidth="1"/>
-    <col min="2" max="6" width="13.7109375" style="45" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="26.69921875" style="27" customWidth="1"/>
+    <col min="2" max="6" width="13.69921875" style="45" customWidth="1"/>
+    <col min="7" max="16384" width="9.09765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -5194,7 +5201,7 @@
       <c r="H1" s="35"/>
       <c r="I1" s="35"/>
     </row>
-    <row r="2" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="9.75" customHeight="1">
       <c r="A2" s="47" t="s">
         <v>46</v>
       </c>
@@ -5204,7 +5211,7 @@
       <c r="E2" s="47"/>
       <c r="F2" s="47"/>
     </row>
-    <row r="3" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="9.9" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -5212,7 +5219,7 @@
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="9.9" customHeight="1">
       <c r="A4" s="37"/>
       <c r="B4" s="49" t="s">
         <v>47</v>
@@ -5224,7 +5231,7 @@
       <c r="E4" s="49"/>
       <c r="F4" s="49"/>
     </row>
-    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="36" customHeight="1">
       <c r="A5" s="38" t="s">
         <v>49</v>
       </c>
@@ -5244,7 +5251,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="9.9" customHeight="1">
       <c r="A6" s="32"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
@@ -5252,7 +5259,7 @@
       <c r="E6" s="40"/>
       <c r="F6" s="40"/>
     </row>
-    <row r="7" spans="1:9" s="17" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="17" customFormat="1" ht="9.9" customHeight="1">
       <c r="A7" s="33" t="s">
         <v>5</v>
       </c>
@@ -5272,7 +5279,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="9.9" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -5280,7 +5287,7 @@
       <c r="E8" s="40"/>
       <c r="F8" s="40"/>
     </row>
-    <row r="9" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="9.9" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>6</v>
       </c>
@@ -5300,7 +5307,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="9.9" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="40"/>
       <c r="C10" s="40"/>
@@ -5308,7 +5315,7 @@
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
     </row>
-    <row r="11" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="9.9" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>7</v>
       </c>
@@ -5328,7 +5335,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="9.9" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>8</v>
       </c>
@@ -5348,7 +5355,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="9.9" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>9</v>
       </c>
@@ -5368,7 +5375,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="9.9" customHeight="1">
       <c r="A14" s="32" t="s">
         <v>10</v>
       </c>
@@ -5388,7 +5395,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="9.9" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>11</v>
       </c>
@@ -5408,7 +5415,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="9.9" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>12</v>
       </c>
@@ -5428,7 +5435,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="9.9" customHeight="1">
       <c r="A17" s="32" t="s">
         <v>13</v>
       </c>
@@ -5448,7 +5455,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="9.9" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>14</v>
       </c>
@@ -5468,7 +5475,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="9.9" customHeight="1">
       <c r="A19" s="32" t="s">
         <v>15</v>
       </c>
@@ -5488,7 +5495,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="9.9" customHeight="1">
       <c r="A20" s="32" t="s">
         <v>16</v>
       </c>
@@ -5508,7 +5515,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="9.9" customHeight="1">
       <c r="A21" s="32" t="s">
         <v>17</v>
       </c>
@@ -5528,7 +5535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="9.9" customHeight="1">
       <c r="A22" s="32" t="s">
         <v>18</v>
       </c>
@@ -5548,7 +5555,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="9.9" customHeight="1">
       <c r="A23" s="32" t="s">
         <v>19</v>
       </c>
@@ -5568,7 +5575,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="9.9" customHeight="1">
       <c r="A24" s="32" t="s">
         <v>20</v>
       </c>
@@ -5588,7 +5595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="9.9" customHeight="1">
       <c r="A25" s="32" t="s">
         <v>21</v>
       </c>
@@ -5608,7 +5615,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="9.9" customHeight="1">
       <c r="A26" s="32" t="s">
         <v>22</v>
       </c>
@@ -5628,7 +5635,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="9.9" customHeight="1">
       <c r="A27" s="32" t="s">
         <v>23</v>
       </c>
@@ -5648,7 +5655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="9.9" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -5656,7 +5663,7 @@
       <c r="E28" s="40"/>
       <c r="F28" s="40"/>
     </row>
-    <row r="29" spans="1:6" s="17" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="17" customFormat="1" ht="9.9" customHeight="1">
       <c r="A29" s="33" t="s">
         <v>24</v>
       </c>
@@ -5676,7 +5683,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="9.9" customHeight="1">
       <c r="A30" s="32"/>
       <c r="B30" s="40"/>
       <c r="C30" s="40"/>
@@ -5684,7 +5691,7 @@
       <c r="E30" s="40"/>
       <c r="F30" s="40"/>
     </row>
-    <row r="31" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="9.9" customHeight="1">
       <c r="A31" s="32" t="s">
         <v>6</v>
       </c>
@@ -5704,7 +5711,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="9.9" customHeight="1">
       <c r="A32" s="32" t="s">
         <v>27</v>
       </c>
@@ -5724,7 +5731,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="9.9" customHeight="1">
       <c r="A33" s="32" t="s">
         <v>28</v>
       </c>
@@ -5744,7 +5751,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="9.9" customHeight="1">
       <c r="A34" s="32"/>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
@@ -5752,7 +5759,7 @@
       <c r="E34" s="40"/>
       <c r="F34" s="40"/>
     </row>
-    <row r="35" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="9.9" customHeight="1">
       <c r="A35" s="32" t="s">
         <v>7</v>
       </c>
@@ -5772,7 +5779,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="9.9" customHeight="1">
       <c r="A36" s="32" t="s">
         <v>8</v>
       </c>
@@ -5792,7 +5799,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="9.9" customHeight="1">
       <c r="A37" s="32" t="s">
         <v>9</v>
       </c>
@@ -5812,7 +5819,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="9.9" customHeight="1">
       <c r="A38" s="32" t="s">
         <v>10</v>
       </c>
@@ -5832,7 +5839,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="9.9" customHeight="1">
       <c r="A39" s="32" t="s">
         <v>29</v>
       </c>
@@ -5852,7 +5859,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="9.9" customHeight="1">
       <c r="A40" s="32" t="s">
         <v>12</v>
       </c>
@@ -5872,7 +5879,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="9.9" customHeight="1">
       <c r="A41" s="32" t="s">
         <v>13</v>
       </c>
@@ -5892,7 +5899,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="9.9" customHeight="1">
       <c r="A42" s="32" t="s">
         <v>31</v>
       </c>
@@ -5912,7 +5919,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="9.9" customHeight="1">
       <c r="A43" s="32" t="s">
         <v>16</v>
       </c>
@@ -5932,7 +5939,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="9.9" customHeight="1">
       <c r="A44" s="32" t="s">
         <v>17</v>
       </c>
@@ -5952,7 +5959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="9.9" customHeight="1">
       <c r="A45" s="32" t="s">
         <v>18</v>
       </c>
@@ -5972,7 +5979,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="9.9" customHeight="1">
       <c r="A46" s="32" t="s">
         <v>55</v>
       </c>
@@ -5992,7 +5999,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="9.9" customHeight="1">
       <c r="A47" s="32"/>
       <c r="B47" s="40"/>
       <c r="C47" s="40"/>
@@ -6000,7 +6007,7 @@
       <c r="E47" s="40"/>
       <c r="F47" s="40"/>
     </row>
-    <row r="48" spans="1:6" s="17" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="17" customFormat="1" ht="9.9" customHeight="1">
       <c r="A48" s="33" t="s">
         <v>34</v>
       </c>
@@ -6020,7 +6027,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="9.9" customHeight="1">
       <c r="A49" s="32"/>
       <c r="B49" s="40"/>
       <c r="C49" s="40"/>
@@ -6028,7 +6035,7 @@
       <c r="E49" s="40"/>
       <c r="F49" s="40"/>
     </row>
-    <row r="50" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="9.9" customHeight="1">
       <c r="A50" s="32" t="s">
         <v>6</v>
       </c>
@@ -6048,7 +6055,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="9.9" customHeight="1">
       <c r="A51" s="32"/>
       <c r="B51" s="40"/>
       <c r="C51" s="40"/>
@@ -6056,7 +6063,7 @@
       <c r="E51" s="40"/>
       <c r="F51" s="40"/>
     </row>
-    <row r="52" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="9.9" customHeight="1">
       <c r="A52" s="32" t="s">
         <v>7</v>
       </c>
@@ -6076,7 +6083,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="9.9" customHeight="1">
       <c r="A53" s="32" t="s">
         <v>9</v>
       </c>
@@ -6096,7 +6103,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="9.9" customHeight="1">
       <c r="A54" s="32" t="s">
         <v>10</v>
       </c>
@@ -6116,7 +6123,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="9.9" customHeight="1">
       <c r="A55" s="32" t="s">
         <v>29</v>
       </c>
@@ -6136,7 +6143,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="9.9" customHeight="1">
       <c r="A56" s="32" t="s">
         <v>12</v>
       </c>
@@ -6156,7 +6163,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="9.9" customHeight="1">
       <c r="A57" s="32" t="s">
         <v>14</v>
       </c>
@@ -6176,7 +6183,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="9.9" customHeight="1">
       <c r="A58" s="32" t="s">
         <v>15</v>
       </c>
@@ -6196,7 +6203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="9.9" customHeight="1">
       <c r="A59" s="32" t="s">
         <v>16</v>
       </c>
@@ -6216,7 +6223,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="9.9" customHeight="1">
       <c r="A60" s="32" t="s">
         <v>18</v>
       </c>
@@ -6236,7 +6243,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="9.9" customHeight="1">
       <c r="A61" s="32" t="s">
         <v>36</v>
       </c>
@@ -6256,7 +6263,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="9.9" customHeight="1">
       <c r="A62" s="32" t="s">
         <v>20</v>
       </c>
@@ -6276,7 +6283,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="9.9" customHeight="1">
       <c r="A63" s="32" t="s">
         <v>33</v>
       </c>
@@ -6296,7 +6303,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="9.9" customHeight="1">
       <c r="A64" s="19" t="s">
         <v>37</v>
       </c>
@@ -6316,8 +6323,8 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="7.5" customHeight="1"/>
+    <row r="66" spans="1:6" ht="9.9" customHeight="1">
       <c r="A66" s="22" t="s">
         <v>56</v>
       </c>
@@ -6327,7 +6334,7 @@
       <c r="E66" s="22"/>
       <c r="F66" s="22"/>
     </row>
-    <row r="67" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="7.5" customHeight="1">
       <c r="A67" s="22"/>
       <c r="B67" s="43"/>
       <c r="C67" s="43"/>
@@ -6335,9 +6342,9 @@
       <c r="E67" s="43"/>
       <c r="F67" s="43"/>
     </row>
-    <row r="68" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="9.9" customHeight="1">
       <c r="A68" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
@@ -6345,7 +6352,7 @@
       <c r="E68" s="22"/>
       <c r="F68" s="22"/>
     </row>
-    <row r="69" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="9.9" customHeight="1">
       <c r="A69" s="1" t="s">
         <v>45</v>
       </c>
@@ -6355,8 +6362,8 @@
       <c r="E69" s="22"/>
       <c r="F69" s="22"/>
     </row>
-    <row r="70" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:6" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="7.5" customHeight="1"/>
+    <row r="71" spans="1:6" ht="9.9" customHeight="1">
       <c r="A71" s="50" t="s">
         <v>57</v>
       </c>
@@ -6375,7 +6382,7 @@
     <mergeCell ref="D4:F4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A69" r:id="rId1" tooltip="&lt;www.census.gov/construction/c30/meth.html&gt;" xr:uid="{28C06CA1-3342-45F6-8771-E5A84F6E79A3}"/>
+    <hyperlink ref="A69" r:id="rId1" tooltip="&lt;www.census.gov/construction/c30/meth.html&gt;"/>
   </hyperlinks>
   <pageMargins left="0.55555555555555602" right="0.27777777777777801" top="0.41666666666666702" bottom="0.13888888888888901" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -6383,32 +6390,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF533741-6009-4019-AB40-EF61A70F48B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="9.9" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="44" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="25" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" style="26" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="26.69921875" style="44" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="14.69921875" style="25" customWidth="1"/>
+    <col min="4" max="5" width="14.69921875" style="26" customWidth="1"/>
+    <col min="6" max="16384" width="9.09765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13.8">
       <c r="A1" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
     </row>
-    <row r="2" spans="1:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="9.75" customHeight="1">
       <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
@@ -6417,14 +6424,14 @@
       <c r="D2" s="47"/>
       <c r="E2" s="47"/>
     </row>
-    <row r="3" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="9.9" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="21.9" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -6441,14 +6448,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="8.25" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" s="17" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="17" customFormat="1" ht="9.9" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
@@ -6465,14 +6472,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="4.5" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="9.9" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -6489,14 +6496,14 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="4.5" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="9.9" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -6513,7 +6520,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="9.9" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -6530,7 +6537,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="9.9" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -6547,7 +6554,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="9.9" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -6564,7 +6571,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="9.9" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -6581,7 +6588,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="9.9" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -6598,7 +6605,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="9.9" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -6615,7 +6622,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="9.9" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -6632,7 +6639,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="9.9" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -6649,7 +6656,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="9.9" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -6666,7 +6673,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="9.9" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -6683,7 +6690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="9.9" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -6700,7 +6707,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="9.9" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -6717,7 +6724,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="9.9" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -6734,7 +6741,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="9.9" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -6751,7 +6758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="9.9" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
@@ -6768,7 +6775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="9.9" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -6785,14 +6792,14 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="4.5" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="1:5" s="17" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="17" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="14" t="s">
         <v>25</v>
       </c>
@@ -6809,14 +6816,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="4.5" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
     </row>
-    <row r="30" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="12" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
@@ -6833,7 +6840,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="9.9" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
@@ -6850,7 +6857,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="9.9" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
@@ -6867,14 +6874,14 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="4.5" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
     </row>
-    <row r="34" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="9.9" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -6891,7 +6898,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="9.9" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
@@ -6908,7 +6915,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="9.9" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>9</v>
       </c>
@@ -6925,7 +6932,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="9.9" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -6942,7 +6949,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="9.9" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>29</v>
       </c>
@@ -6959,7 +6966,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="9.9" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>12</v>
       </c>
@@ -6976,7 +6983,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="9.9" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>13</v>
       </c>
@@ -6993,7 +7000,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="9.9" customHeight="1">
       <c r="A41" s="3" t="s">
         <v>14</v>
       </c>
@@ -7010,7 +7017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="9.9" customHeight="1">
       <c r="A42" s="3" t="s">
         <v>31</v>
       </c>
@@ -7027,7 +7034,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="9.9" customHeight="1">
       <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
@@ -7044,7 +7051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="9.9" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>17</v>
       </c>
@@ -7061,7 +7068,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="9.9" customHeight="1">
       <c r="A45" s="3" t="s">
         <v>18</v>
       </c>
@@ -7078,7 +7085,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="9.9" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>32</v>
       </c>
@@ -7095,7 +7102,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="9.9" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>33</v>
       </c>
@@ -7112,7 +7119,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="9.9" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>23</v>
       </c>
@@ -7129,14 +7136,14 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="4.5" customHeight="1">
       <c r="A49" s="3"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
     </row>
-    <row r="50" spans="1:5" s="17" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" s="17" customFormat="1" ht="12" customHeight="1">
       <c r="A50" s="14" t="s">
         <v>35</v>
       </c>
@@ -7153,14 +7160,14 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="4.5" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
     </row>
-    <row r="52" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="9.9" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>6</v>
       </c>
@@ -7177,14 +7184,14 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="4.5" customHeight="1">
       <c r="A53" s="3"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
     </row>
-    <row r="54" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="9.9" customHeight="1">
       <c r="A54" s="3" t="s">
         <v>7</v>
       </c>
@@ -7201,7 +7208,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="9.9" customHeight="1">
       <c r="A55" s="3" t="s">
         <v>9</v>
       </c>
@@ -7218,7 +7225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="9.9" customHeight="1">
       <c r="A56" s="3" t="s">
         <v>10</v>
       </c>
@@ -7235,7 +7242,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="9.9" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>29</v>
       </c>
@@ -7252,7 +7259,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="9.9" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>12</v>
       </c>
@@ -7269,7 +7276,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="9.9" customHeight="1">
       <c r="A59" s="3" t="s">
         <v>14</v>
       </c>
@@ -7286,7 +7293,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="9.9" customHeight="1">
       <c r="A60" s="3" t="s">
         <v>15</v>
       </c>
@@ -7303,7 +7310,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="9.9" customHeight="1">
       <c r="A61" s="3" t="s">
         <v>16</v>
       </c>
@@ -7320,7 +7327,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="9.9" customHeight="1">
       <c r="A62" s="3" t="s">
         <v>18</v>
       </c>
@@ -7337,7 +7344,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="9.9" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>36</v>
       </c>
@@ -7354,7 +7361,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="9.9" customHeight="1">
       <c r="A64" s="3" t="s">
         <v>20</v>
       </c>
@@ -7371,7 +7378,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="9.9" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>33</v>
       </c>
@@ -7388,7 +7395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" ht="9.9" customHeight="1">
       <c r="A66" s="19" t="s">
         <v>37</v>
       </c>
@@ -7405,8 +7412,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="4.5" customHeight="1"/>
+    <row r="68" spans="1:5" ht="9.9" customHeight="1">
       <c r="A68" s="22" t="s">
         <v>38</v>
       </c>
@@ -7415,14 +7422,14 @@
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
     </row>
-    <row r="69" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="4.5" customHeight="1">
       <c r="A69" s="22"/>
       <c r="B69" s="22"/>
       <c r="C69" s="22"/>
       <c r="D69" s="22"/>
       <c r="E69" s="22"/>
     </row>
-    <row r="70" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="12" customHeight="1">
       <c r="A70" s="23" t="s">
         <v>39</v>
       </c>
@@ -7431,7 +7438,7 @@
       <c r="D70" s="23"/>
       <c r="E70" s="23"/>
     </row>
-    <row r="71" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="9.9" customHeight="1">
       <c r="A71" s="22" t="s">
         <v>40</v>
       </c>
@@ -7440,14 +7447,14 @@
       <c r="D71" s="22"/>
       <c r="E71" s="22"/>
     </row>
-    <row r="72" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="4.5" customHeight="1">
       <c r="A72" s="22"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
       <c r="D72" s="22"/>
       <c r="E72" s="22"/>
     </row>
-    <row r="73" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="12" customHeight="1">
       <c r="A73" s="23" t="s">
         <v>41</v>
       </c>
@@ -7456,14 +7463,14 @@
       <c r="D73" s="23"/>
       <c r="E73" s="23"/>
     </row>
-    <row r="74" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="4.5" customHeight="1">
       <c r="A74" s="22"/>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
       <c r="E74" s="22"/>
     </row>
-    <row r="75" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" ht="12" customHeight="1">
       <c r="A75" s="22" t="s">
         <v>42</v>
       </c>
@@ -7472,7 +7479,7 @@
       <c r="D75" s="22"/>
       <c r="E75" s="22"/>
     </row>
-    <row r="76" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="9.9" customHeight="1">
       <c r="A76" s="22" t="s">
         <v>43</v>
       </c>
@@ -7481,19 +7488,19 @@
       <c r="D76" s="22"/>
       <c r="E76" s="22"/>
     </row>
-    <row r="77" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="4.5" customHeight="1">
       <c r="A77" s="2"/>
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
       <c r="E77" s="22"/>
     </row>
-    <row r="78" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="9.9" customHeight="1">
       <c r="A78" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="9.9" customHeight="1">
       <c r="A79" s="22" t="s">
         <v>45</v>
       </c>
@@ -7504,7 +7511,7 @@
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A79" r:id="rId1" tooltip="&lt;www.census.gov/construction/c30/meth.html&gt;" xr:uid="{4B41EBA4-7F14-4ABD-A3C7-6800124A97CE}"/>
+    <hyperlink ref="A79" r:id="rId1" tooltip="&lt;www.census.gov/construction/c30/meth.html&gt;"/>
   </hyperlinks>
   <pageMargins left="0.69444444444444442" right="0.55555555555555558" top="0.41666666666666669" bottom="0.1388888888888889" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>